<commit_message>
Account Payables Test Plans
</commit_message>
<xml_diff>
--- a/templates/POLOADER.xlsx
+++ b/templates/POLOADER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ERPFinalProj\rsqasampleproj\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dellDevonforce\Provar\ErpFinalProject\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBC3967-2B6E-48FD-A095-0265EB24C065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1171EB90-40BA-4673-B4ED-A778FEA5EA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{B6C21A89-21B4-4624-A955-66D166717697}"/>
   </bookViews>
   <sheets>
     <sheet name="AddBoth" sheetId="15" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="52">
   <si>
     <t>Vendor</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>a1E1K000008NTam</t>
+  </si>
+  <si>
+    <t>AsynchronousProcessing</t>
+  </si>
+  <si>
+    <t>a3Z1K0000008Bhe</t>
   </si>
 </sst>
 </file>
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D721CDB-A9DB-40A7-92FA-BE728EC43FA8}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +739,124 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>411002</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>200.55</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5">
+        <v>411002</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>200.55</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -740,10 +864,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC89EBC-4F44-4337-884E-CD4887F2A248}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,6 +1058,130 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4">
+        <v>411002</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>1500</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5">
+        <v>411002</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>2460</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -941,13 +1189,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7DA735-ABAD-4CED-8CC9-BD6A39927EAB}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1010,6 +1261,38 @@
         <v>200.55</v>
       </c>
       <c r="J2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>200.55</v>
+      </c>
+      <c r="J3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1020,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA76DEB8-C288-4FFF-933C-5D83C119E0BF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,6 +1343,20 @@
         <v>33</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1070,7 +1367,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D68A558F-1570-4CED-A748-7B569825A34D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,6 +1488,29 @@
         <v>15.897</v>
       </c>
       <c r="G2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>15.897</v>
+      </c>
+      <c r="G3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1204,7 +1524,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559F99DE-9B6A-4DC2-AFC0-6B79DDA70449}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1619,7 @@
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1333,8 +1653,11 @@
       <c r="K1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1368,8 +1691,11 @@
       <c r="K2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1402,6 +1728,85 @@
       </c>
       <c r="K3" t="s">
         <v>22</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>411011</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5">
+        <v>411018</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1411,16 +1816,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BAAF839-3C85-47A3-8C0F-A4F8E32EA17E}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:Q3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -1606,6 +2012,130 @@
         <v>24</v>
       </c>
       <c r="T3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4">
+        <v>400056</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5">
+        <v>400056</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <v>1000</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1616,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D1DF1B-CADC-480B-9F9D-24CB1D04E075}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,6 +2277,88 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>2000</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>250</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>